<commit_message>
More column tidying. Gallery1_X populated
</commit_message>
<xml_diff>
--- a/Wireframes.xlsx
+++ b/Wireframes.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
-  <si>
-    <t>Wireframe for scrolling gallery</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>1/#</t>
   </si>
@@ -90,25 +87,184 @@
     <t>nav HIDDEN ATM</t>
   </si>
   <si>
-    <t>gallery</t>
-  </si>
-  <si>
-    <r>
-      <t>thumbnails un</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ordered list styled to arrange horizontally</t>
-    </r>
-  </si>
-  <si>
     <t>&lt;links</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">thumbnails </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unordered list styled to arrange horizontally</t>
+    </r>
+  </si>
+  <si>
+    <t>Gallery</t>
+  </si>
+  <si>
+    <t>Portfolio</t>
+  </si>
+  <si>
+    <t>nav</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Portfolio Title </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+  </si>
+  <si>
+    <t>Thumb</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Title 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>h2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Title 3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>h2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Title 4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>h2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Title 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>h2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Details </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>h2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Title 5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>h2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Title 6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>h2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Title 7 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>h2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Title 8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>h2</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -145,7 +301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -341,59 +497,127 @@
         <color indexed="64"/>
       </diagonal>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,136 +919,289 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="30"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="33"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="31"/>
+      <c r="C4" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="34"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="31"/>
+      <c r="C5" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="34"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="31"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="34"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="31"/>
+      <c r="C7" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="32"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="35"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="31"/>
+      <c r="C9" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="34"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="31"/>
+      <c r="C10" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="34"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="31"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="34"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="36"/>
+      <c r="C12" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="37"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="25"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="22"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="25" t="s">
-        <v>14</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="D6:E9"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D10:E10"/>
+  <mergeCells count="14">
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F10:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>